<commit_message>
Feito o calendário para o plano de fidelidade
</commit_message>
<xml_diff>
--- a/Material/timesheet.xlsx
+++ b/Material/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Dia</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Evolução das telas de pedido. (Reorganização e definição de todos os estados/regras)</t>
+  </si>
+  <si>
+    <t>Ponta-pé inicial da parte de fidelidade do sistema</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,10 +517,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="1">
+        <v>42619</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.875</v>
+      </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tela do fidelidade finalizada. Falta terminar o consultar, excluir e alterar.
</commit_message>
<xml_diff>
--- a/Material/timesheet.xlsx
+++ b/Material/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Dia</t>
   </si>
@@ -47,7 +47,10 @@
     <t>Evolução das telas de pedido. (Reorganização e definição de todos os estados/regras)</t>
   </si>
   <si>
-    <t>Ponta-pé inicial da parte de fidelidade do sistema</t>
+    <t>Ponta-pé inicial da parte de fidelidade do sistema(Tela e definições básicas)</t>
+  </si>
+  <si>
+    <t>Definição final sobre o funcionamento da fidelidade</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,17 +526,25 @@
       <c r="B3" s="2">
         <v>0.875</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="1">
+        <v>42622</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Feito o login (utilizando sessionStorage e redirecionando para pedidos_abertos)
</commit_message>
<xml_diff>
--- a/Material/timesheet.xlsx
+++ b/Material/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Dia</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Definição final sobre o funcionamento da fidelidade</t>
+  </si>
+  <si>
+    <t>Estudo e implantação do sessionStorage + login</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,10 +551,18 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="1">
+        <v>42626</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Entrega do cadastrar cliente
</commit_message>
<xml_diff>
--- a/Material/timesheet.xlsx
+++ b/Material/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Dia</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Estudo e implantação do sessionStorage + login</t>
+  </si>
+  <si>
+    <t>Implementação do cadastrar cliente</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,10 +569,18 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="1">
+        <v>42627</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajuste no redirecionamento após a criação de um novo usuário
</commit_message>
<xml_diff>
--- a/Material/timesheet.xlsx
+++ b/Material/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Dia</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Implementação do cadastrar cliente</t>
+  </si>
+  <si>
+    <t>Implementação do login com ramificação. Implementação do CRUD de motoboy</t>
+  </si>
+  <si>
+    <t>Estudo e tentativa de confirmação para exclusão da conta do cliente</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,17 +590,33 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="1">
+        <v>42627</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="1">
+        <v>42627</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alteração no timesheet e no txt de Definições do sistema
</commit_message>
<xml_diff>
--- a/Material/timesheet.xlsx
+++ b/Material/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Dia</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Estudo e tentativa de confirmação para exclusão da conta do cliente</t>
+  </si>
+  <si>
+    <t>Implementação das tarefas (kanbanflow) do dia 28/09</t>
   </si>
 </sst>
 </file>
@@ -486,14 +489,14 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,10 +623,18 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="1">
+        <v>42641</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uma marmitex pode ter N ingredientes repetidos
</commit_message>
<xml_diff>
--- a/Material/timesheet.xlsx
+++ b/Material/timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Dia</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Implementação das tarefas (kanbanflow) do dia 28/09</t>
+  </si>
+  <si>
+    <t>Implementação do pagamento por Créditos</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,10 +641,18 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="1">
+        <v>42646</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>